<commit_message>
[feat]: Add benchmark script
</commit_message>
<xml_diff>
--- a/Imbalance Benchmark.xlsx
+++ b/Imbalance Benchmark.xlsx
@@ -1493,92 +1493,62 @@
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>72.330 (1.217)</t>
+          <t>80.030 (0.646)</t>
         </is>
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>64.699 (1.630)</t>
+          <t>76.116 (0.889)</t>
         </is>
       </c>
       <c r="D6" s="6" t="inlineStr">
         <is>
-          <t>64.335 (2.545)</t>
+          <t>76.418 (1.255)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>81.110 (0.489)</t>
+          <t>84.970 (0.527)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>77.426 (0.466)</t>
+          <t>82.680 (0.728)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>78.527 (0.579)</t>
+          <t>83.301 (0.667)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>54.990 (1.000)</t>
+          <t>64.710 (0.803)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>48.458 (0.949)</t>
+          <t>58.119 (0.733)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>43.434 (1.230)</t>
+          <t>51.492 (1.577)</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>69.850 (0.636)</t>
+          <t>70.960 (0.450)</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>63.212 (0.822)</t>
+          <t>64.043 (0.501)</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>62.497 (1.220)</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>53.120 (0.839)</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>43.354 (0.677)</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>36.547 (0.938)</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>76.160 (0.776)</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>68.321 (1.361)</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>69.765 (1.653)</t>
+          <t>60.787 (0.863)</t>
         </is>
       </c>
     </row>
@@ -1783,6 +1753,36 @@
       <c r="M12" t="inlineStr">
         <is>
           <t>67.518 (0.550)</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>67.900 (2.106)</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>65.440 (3.259)</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>64.121 (2.769)</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>80.200 (0.346)</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>77.456 (0.460)</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>77.953 (0.362)</t>
         </is>
       </c>
     </row>
@@ -1922,47 +1922,47 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>40.236 (0.246)</t>
+          <t>90.933 (0.159)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>46.773 (0.122)</t>
+          <t>83.850 (0.553)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>30.392 (0.655)</t>
+          <t>83.799 (0.841)</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>59.613 (1.875)</t>
+          <t>72.892 (3.246)</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>42.245 (1.002)</t>
+          <t>36.448 (7.049)</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>31.268 (1.680)</t>
+          <t>33.942 (7.430)</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>33.851 (0.451)</t>
+          <t>92.796 (0.091)</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>47.117 (0.730)</t>
+          <t>88.617 (0.233)</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>22.937 (0.533)</t>
+          <t>89.867 (0.179)</t>
         </is>
       </c>
     </row>
@@ -1979,6 +1979,51 @@
           <t>GraphSMOTE 21'</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>91.534 (0.274)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>86.850 (0.520)</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>88.133 (0.511)</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>71.735 (1.678)</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>40.059 (1.465)</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>37.582 (1.500)</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>92.450 (0.084)</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>87.804 (0.243)</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>89.186 (0.194)</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="inlineStr">
@@ -1995,32 +2040,47 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>84.525 (0.545)</t>
+          <t>90.961 (0.396)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>87.164 (0.637)</t>
+          <t>91.290 (0.150)</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>82.242 (0.450)</t>
+          <t>88.617 (0.373)</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>75.000 (0.939)</t>
+          <t>82.284 (0.812)</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>81.585 (0.520)</t>
+          <t>87.639 (0.231)</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>72.979 (0.904)</t>
+          <t>79.302 (0.672)</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>92.172 (0.225)</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>90.492 (0.177)</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>85.814 (3.212)</t>
         </is>
       </c>
     </row>
@@ -2051,34 +2111,49 @@
           <t>GraphSHA 23‘</t>
         </is>
       </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>92.112 (0.176)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>91.075 (0.149)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>89.862 (0.165)</t>
+        </is>
+      </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>74.404 (0.518)</t>
+          <t>84.051 (0.403)</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>74.952 (0.307)</t>
+          <t>84.767 (0.537)</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>64.739 (0.723)</t>
+          <t>81.291 (0.436)</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>83.468 (0.449)</t>
+          <t>92.533 (0.060)</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>84.553 (0.364)</t>
+          <t>90.140 (0.143)</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>74.560 (2.376)</t>
+          <t>84.724 (2.489)</t>
         </is>
       </c>
     </row>

</xml_diff>